<commit_message>
Add tags to models
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/Chado-Model.xlsx
+++ b/molgenis-model-registry/src/test/resources/Chado-Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="34540" yWindow="1100" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
@@ -2201,9 +2201,6 @@
     <t>Publication</t>
   </si>
   <si>
-    <t>chado_home,chado_pub1</t>
-  </si>
-  <si>
     <t>chado_biosharing</t>
   </si>
   <si>
@@ -2211,6 +2208,9 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>chado_home,chado_pub1,chado_biosharing</t>
   </si>
 </sst>
 </file>
@@ -2271,8 +2271,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2294,7 +2296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2303,6 +2305,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2311,6 +2314,7 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2642,11 +2646,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="37.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -2667,7 +2674,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
     </row>
   </sheetData>
@@ -20590,15 +20597,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" customWidth="1"/>
+    <col min="2" max="3" width="89.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -20665,16 +20671,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>713</v>
+      </c>
+      <c r="B4" t="s">
         <v>714</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>714</v>
+      </c>
+      <c r="D4" t="s">
         <v>715</v>
-      </c>
-      <c r="C4" t="s">
-        <v>715</v>
-      </c>
-      <c r="D4" t="s">
-        <v>716</v>
       </c>
       <c r="E4" t="s">
         <v>704</v>

</xml_diff>